<commit_message>
fin migracion. falta revisar si esta bien encarada la ultima parte pero x lo pronto ya estan todos los datos migrados..
</commit_message>
<xml_diff>
--- a/datos base original.xlsx
+++ b/datos base original.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\backup\UTN\Gestion de datos\TP Hotel Frba 1.0 - 1C 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\gdd2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE65C0A-8AE3-4ADF-98F9-9CEF9325BA2E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC5D556-1D4E-4D0A-A980-95DC988989D1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{FCF5B732-F3D5-49A8-B838-E4A3064B623E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="255">
   <si>
     <t>HabitacionTipoPorcentual</t>
   </si>
@@ -719,14 +720,94 @@
   </si>
   <si>
     <t>Hay pasaportes duplicados</t>
+  </si>
+  <si>
+    <t>Si consumible no tiene cod desc y precio-&gt; precio habitacion</t>
+  </si>
+  <si>
+    <t>si tiene-&gt; precio item (?)</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>est f inicio</t>
+  </si>
+  <si>
+    <t>est cant noche</t>
+  </si>
+  <si>
+    <t>cons codig</t>
+  </si>
+  <si>
+    <t>cons desc</t>
+  </si>
+  <si>
+    <t>cons pre</t>
+  </si>
+  <si>
+    <t>item fact cant</t>
+  </si>
+  <si>
+    <t>item fac mont</t>
+  </si>
+  <si>
+    <t>fact nro</t>
+  </si>
+  <si>
+    <t>fact fech</t>
+  </si>
+  <si>
+    <t>fact total</t>
+  </si>
+  <si>
+    <t>2017-01-11 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2020-07-19 00:00:00.000</t>
+  </si>
+  <si>
+    <t>86264.00</t>
+  </si>
+  <si>
+    <t>Tomo este como el valor base de la habitacion</t>
+  </si>
+  <si>
+    <t>estos 3 son los extras</t>
+  </si>
+  <si>
+    <t>Hay 1 con todo nulo x reserva(lo descarto, lo tomo como el dia q se hizo la reserva)</t>
+  </si>
+  <si>
+    <t>este q tiene todo nulo - la est cant de noches, tb lo descarto ya q esa info la use en estadia y no modifica la factura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La factura se compone de </t>
+  </si>
+  <si>
+    <t>Item1: ValorBase de la estadia</t>
+  </si>
+  <si>
+    <t>Item2: Valor de la suma de consumibles</t>
+  </si>
+  <si>
+    <t>Solo me iomportan si fact fecha is not null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -766,10 +847,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679DB2D7-AEA6-4958-B5E2-8A69BC4D65E9}">
   <dimension ref="A1:AK59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ19" sqref="AJ19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,6 +2160,9 @@
       <c r="O16" t="s">
         <v>93</v>
       </c>
+      <c r="R16" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2100,24 +2185,6 @@
       <c r="O18" t="s">
         <v>95</v>
       </c>
-      <c r="AB18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="G19">
@@ -2176,6 +2243,7 @@
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>155</v>
       </c>
@@ -2213,6 +2281,75 @@
         <v>155</v>
       </c>
       <c r="N23" t="s">
+        <v>155</v>
+      </c>
+      <c r="O23" t="s">
+        <v>155</v>
+      </c>
+      <c r="P23" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>155</v>
+      </c>
+      <c r="R23" t="s">
+        <v>155</v>
+      </c>
+      <c r="S23" t="s">
+        <v>155</v>
+      </c>
+      <c r="T23" t="s">
+        <v>155</v>
+      </c>
+      <c r="U23" t="s">
+        <v>155</v>
+      </c>
+      <c r="V23" t="s">
+        <v>155</v>
+      </c>
+      <c r="W23" t="s">
+        <v>155</v>
+      </c>
+      <c r="X23" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK23" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2240,10 +2377,16 @@
       <c r="A30" t="s">
         <v>189</v>
       </c>
+      <c r="P30" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>190</v>
+      </c>
+      <c r="P31" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -2797,4 +2940,518 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8E0A0F-197E-47FF-A5B3-6ADF7CAAE590}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2326</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2">
+        <v>2396745</v>
+      </c>
+      <c r="J2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2326</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3">
+        <v>2396745</v>
+      </c>
+      <c r="J3" t="s">
+        <v>244</v>
+      </c>
+      <c r="K3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>2325</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>2396745</v>
+      </c>
+      <c r="J4" t="s">
+        <v>244</v>
+      </c>
+      <c r="K4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10001</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10001</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7">
+        <v>850</v>
+      </c>
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7">
+        <v>2396745</v>
+      </c>
+      <c r="J7" t="s">
+        <v>244</v>
+      </c>
+      <c r="K7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>96264</v>
+      </c>
+      <c r="B12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12">
+        <v>190</v>
+      </c>
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12">
+        <v>2473510</v>
+      </c>
+      <c r="J12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>96264</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>2326</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13">
+        <v>2473510</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>96264</v>
+      </c>
+      <c r="B14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>2326</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14">
+        <v>2473510</v>
+      </c>
+      <c r="J14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>96264</v>
+      </c>
+      <c r="B15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>2326</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15">
+        <v>2473510</v>
+      </c>
+      <c r="J15" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>96264</v>
+      </c>
+      <c r="B16" t="s">
+        <v>245</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>96264</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>251</v>
+      </c>
+      <c r="G21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>